<commit_message>
Test with case working.
</commit_message>
<xml_diff>
--- a/tests/db/Charges.xlsx
+++ b/tests/db/Charges.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Admin\Information_Technology\MuniEntry_Files\MuniEntry_app\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37580C51-93CD-4363-8DFA-80A47690B3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -222,12 +228,6 @@
     <t>M1</t>
   </si>
   <si>
-    <t>Minor Misdemeanor</t>
-  </si>
-  <si>
-    <t>Unclassified Misdemeanor</t>
-  </si>
-  <si>
     <t>Failure to Stop for School Bus</t>
   </si>
   <si>
@@ -255,12 +255,6 @@
     <t>Offense Type</t>
   </si>
   <si>
-    <t>Moving Traffic</t>
-  </si>
-  <si>
-    <t>Non-moving Traffic</t>
-  </si>
-  <si>
     <t>Criminal</t>
   </si>
   <si>
@@ -271,12 +265,60 @@
   </si>
   <si>
     <t>Driving Under Suspension FTA, Fines or Child Support</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
+    <t>Non-moving</t>
+  </si>
+  <si>
+    <t>Physical Control</t>
+  </si>
+  <si>
+    <t>4511.194</t>
+  </si>
+  <si>
+    <t>Criminal Mischief - Victim is Family or Household Member</t>
+  </si>
+  <si>
+    <t>Criminal Mischief M3</t>
+  </si>
+  <si>
+    <t>2909.07</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Criminal Mischief - Risk of Physical Harm</t>
+  </si>
+  <si>
+    <t>2909.07*</t>
+  </si>
+  <si>
+    <t>2909.07**</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>UCM</t>
+  </si>
+  <si>
+    <t>Disorderly Conduct - Persistent</t>
+  </si>
+  <si>
+    <t>2917.11(A)(1)</t>
+  </si>
+  <si>
+    <t>M4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -645,30 +687,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.38671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.38671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.38671875" customWidth="1"/>
+    <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -688,7 +730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -696,13 +738,13 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -710,472 +752,542 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4513.04</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5">
-        <v>4513.04</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B29" s="5">
         <v>4511.21</v>
       </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
+      <c r="B36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tests for databases.
</commit_message>
<xml_diff>
--- a/tests/db/Charges.xlsx
+++ b/tests/db/Charges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\tests\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FDB8DC-8320-4166-9B82-9C6FAAC571A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF77A84-7934-4D81-BE65-48A155A0A2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -731,52 +731,59 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>76</v>
@@ -784,13 +791,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -798,13 +805,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>90</v>
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
@@ -812,13 +819,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
@@ -826,44 +833,44 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>91</v>
       </c>
       <c r="D10" t="s">
         <v>80</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
         <v>80</v>
@@ -871,13 +878,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>80</v>
@@ -885,55 +892,55 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>79</v>
+      <c r="A14" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>91</v>
-      </c>
       <c r="D15" t="s">
         <v>80</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>92</v>
@@ -941,44 +948,44 @@
       <c r="D16" t="s">
         <v>80</v>
       </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4513.04</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="5">
-        <v>4513.04</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -989,41 +996,41 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>80</v>
@@ -1031,13 +1038,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -1045,24 +1052,24 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>91</v>
@@ -1073,24 +1080,27 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>92</v>
@@ -1099,32 +1109,29 @@
         <v>81</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4511.21</v>
       </c>
       <c r="C29" t="s">
         <v>91</v>
@@ -1135,10 +1142,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5">
-        <v>4511.21</v>
+        <v>57</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -1149,10 +1156,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -1163,10 +1170,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -1177,38 +1184,38 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -1219,82 +1226,68 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
         <v>91</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
         <v>80</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="E39" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>